<commit_message>
metadata rename changed some column names
</commit_message>
<xml_diff>
--- a/Assembly/measures.xlsx
+++ b/Assembly/measures.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NotBackedUp\local R dev\idi_exemplar_project\Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NotBackedUp\local R dev\idi_exemplar_project\Assembly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E674DE36-A7F1-4FD0-8DBE-88F57A128117}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288E7C00-C512-445B-8AD7-51CAE901D88C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -174,15 +174,9 @@
     <t>address_descriptors.sql</t>
   </si>
   <si>
-    <t>[IUR2018_V1_00_NAME]</t>
-  </si>
-  <si>
     <t>[ant_region_code]</t>
   </si>
   <si>
-    <t>[SA22018_V1_00]</t>
-  </si>
-  <si>
     <t>[defn_address_descriptors]</t>
   </si>
   <si>
@@ -229,6 +223,12 @@
   </si>
   <si>
     <t>[DL-MAA20XX-YY]</t>
+  </si>
+  <si>
+    <t>[IUR2020_V1_00_NAME]</t>
+  </si>
+  <si>
+    <t>[SA22020_V1_00]</t>
   </si>
 </sst>
 </file>
@@ -570,9 +570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -921,25 +919,25 @@
         <v>43</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="I10" s="1" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>40</v>
@@ -948,7 +946,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -959,25 +957,25 @@
         <v>43</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>17</v>
@@ -986,7 +984,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -997,25 +995,25 @@
         <v>43</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I12" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="J12" t="s">
         <v>17</v>
@@ -1024,36 +1022,36 @@
         <v>0</v>
       </c>
       <c r="L12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13" t="s">
         <v>62</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H13" t="s">
-        <v>64</v>
-      </c>
       <c r="I13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J13" t="s">
         <v>44</v>
@@ -1062,7 +1060,7 @@
         <v>0</v>
       </c>
       <c r="L13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>